<commit_message>
Extracting all metadata & types from xlsx files
</commit_message>
<xml_diff>
--- a/epigraphhub/data/brasil/sinan/metadata/SIFG.xlsx
+++ b/epigraphhub/data/brasil/sinan/metadata/SIFG.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="82">
   <si>
     <t xml:space="preserve">Nome do campo</t>
   </si>
@@ -28,7 +28,7 @@
     <t xml:space="preserve">Campo</t>
   </si>
   <si>
-    <t xml:space="preserve">tipo</t>
+    <t xml:space="preserve">Tipo</t>
   </si>
   <si>
     <t xml:space="preserve">Categorias</t>
@@ -187,54 +187,18 @@
     <t xml:space="preserve">tp_teste1</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1 – Reagente
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">2 - Não reagente
+    <t xml:space="preserve">1 – Reagente
+2 - Não reagente
 3 - Não realizado
 9 – Ignorado</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Refere-se ao resultado </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">do teste não treponêmico
+  </si>
+  <si>
+    <t xml:space="preserve">Refere-se ao resultado do teste não treponêmico
 preconizado para a
 primeira consulta de pré-
 natal. Entende-se como
 teste não treponêmicos o
 VDRL e o RPR;</t>
-    </r>
   </si>
   <si>
     <r>
@@ -255,6 +219,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Aceita apenas os
 códigos listados.</t>
@@ -417,17 +382,7 @@
         <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Microhemaglutination
-</t>
-    </r>
-    <r>
-      <rPr>
-        <i val="true"/>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">Treponema pallidum
+Treponema pallidum
 Assay</t>
     </r>
     <r>
@@ -436,6 +391,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">), TPHA
 (</t>
@@ -447,6 +403,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Treponema pallidum
 Hemaglutination Assay</t>
@@ -457,6 +414,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">),
 ELISA (</t>
@@ -468,6 +426,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Enzyme-Linked
 Immunosorbent Assay</t>
@@ -478,33 +437,9 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="0"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">).</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b val="true"/>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Campo Obrigatório
-</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Aceita apenas os
-códigos listados.</t>
     </r>
   </si>
   <si>
@@ -599,25 +534,8 @@
     <t xml:space="preserve">tp_motivo</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">1 - parceiro não teve
-mais contato com a </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="9.5"/>
-        <color rgb="FF000000"/>
-        <rFont val="Arial"/>
-        <family val="0"/>
-      </rPr>
-      <t xml:space="preserve">gestante.
+    <t xml:space="preserve">1 - parceiro não teve
+mais contato com a gestante.
 2 - parceiro não foi
 comunicado/convoca
 do à us para
@@ -635,7 +553,6 @@
 sorologia não
 reagente.
 6 - outro motivo</t>
-    </r>
   </si>
   <si>
     <t xml:space="preserve">Relata o motivo pelo qual o
@@ -734,7 +651,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="10">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -778,19 +695,6 @@
       <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="9.5"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <i val="true"/>
-      <sz val="9.5"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="7.5"/>
@@ -929,7 +833,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -941,7 +845,7 @@
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="164" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -965,10 +869,10 @@
   <dimension ref="A1:H1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C4" activeCellId="0" sqref="C4"/>
+      <selection pane="topLeft" activeCell="D5" activeCellId="0" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="35.88671875" defaultRowHeight="59.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="35.89453125" defaultRowHeight="59.7" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="1" style="1" width="35.85"/>
   </cols>
@@ -1176,122 +1080,122 @@
         <v>55</v>
       </c>
       <c r="F9" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="G9" s="14" t="s">
         <v>56</v>
-      </c>
-      <c r="G9" s="14" t="s">
-        <v>57</v>
       </c>
       <c r="H9" s="9"/>
     </row>
     <row r="10" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="B10" s="7" t="s">
         <v>58</v>
-      </c>
-      <c r="B10" s="7" t="s">
-        <v>59</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D10" s="7" t="s">
+        <v>59</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>60</v>
       </c>
-      <c r="E10" s="7" t="s">
+      <c r="F10" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G10" s="8" t="s">
         <v>61</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>56</v>
-      </c>
-      <c r="G10" s="8" t="s">
-        <v>62</v>
       </c>
       <c r="H10" s="9"/>
     </row>
     <row r="11" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="B11" s="6" t="s">
         <v>63</v>
-      </c>
-      <c r="B11" s="6" t="s">
-        <v>64</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D11" s="7" t="s">
+        <v>64</v>
+      </c>
+      <c r="E11" s="7" t="s">
         <v>65</v>
-      </c>
-      <c r="E11" s="7" t="s">
-        <v>66</v>
       </c>
       <c r="F11" s="10"/>
       <c r="G11" s="8" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="H11" s="9"/>
     </row>
     <row r="12" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="B12" s="6" t="s">
         <v>68</v>
-      </c>
-      <c r="B12" s="6" t="s">
-        <v>69</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>27</v>
       </c>
       <c r="D12" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E12" s="7" t="s">
         <v>70</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>71</v>
       </c>
       <c r="F12" s="10"/>
       <c r="G12" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H12" s="9"/>
     </row>
     <row r="13" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="B13" s="11" t="s">
         <v>73</v>
-      </c>
-      <c r="B13" s="11" t="s">
-        <v>74</v>
       </c>
       <c r="C13" s="12" t="s">
         <v>27</v>
       </c>
       <c r="D13" s="12" t="s">
+        <v>74</v>
+      </c>
+      <c r="E13" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="E13" s="12" t="s">
-        <v>76</v>
       </c>
       <c r="F13" s="15"/>
       <c r="G13" s="14" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="H13" s="9"/>
     </row>
     <row r="14" customFormat="false" ht="59.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B14" s="11" t="s">
         <v>78</v>
-      </c>
-      <c r="B14" s="11" t="s">
-        <v>79</v>
       </c>
       <c r="C14" s="12" t="s">
         <v>40</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="F14" s="12" t="s">
         <v>80</v>
       </c>
-      <c r="F14" s="12" t="s">
+      <c r="G14" s="14" t="s">
         <v>81</v>
-      </c>
-      <c r="G14" s="14" t="s">
-        <v>82</v>
       </c>
       <c r="H14" s="9"/>
     </row>

</xml_diff>